<commit_message>
All PERMANOVAS, betadispersions and pairwise PERMANOVAS written to tables in excel. Specieslist made and written to excel. Sitelist made and written to excel. PCO figures modified. Species of interest figure modified. KDE figure produced.
</commit_message>
<xml_diff>
--- a/Figures/PERMANOVA_bio_1.xlsx
+++ b/Figures/PERMANOVA_bio_1.xlsx
@@ -229,19 +229,19 @@
         <v>1.0</v>
       </c>
       <c r="C2" t="n">
-        <v>36905.05235770268</v>
+        <v>0.21075711429381644</v>
       </c>
       <c r="D2" t="n">
-        <v>36905.05235770268</v>
+        <v>0.21075711429381644</v>
       </c>
       <c r="E2" t="n">
-        <v>0.3807805780013232</v>
+        <v>0.10134734964029923</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0025436727557067475</v>
+        <v>6.587510490031676E-4</v>
       </c>
       <c r="G2" t="n">
-        <v>0.5607</v>
+        <v>0.7514</v>
       </c>
     </row>
     <row r="3">
@@ -252,19 +252,19 @@
         <v>1.0</v>
       </c>
       <c r="C3" t="n">
-        <v>494450.51352608047</v>
+        <v>19.949309312641933</v>
       </c>
       <c r="D3" t="n">
-        <v>494450.51352608047</v>
+        <v>19.949309312641933</v>
       </c>
       <c r="E3" t="n">
-        <v>5.101663330771986</v>
+        <v>9.593078899211893</v>
       </c>
       <c r="F3" t="n">
-        <v>0.03407989475562944</v>
+        <v>0.06235437641393587</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0131</v>
+        <v>0.0017</v>
       </c>
     </row>
     <row r="4">
@@ -275,19 +275,19 @@
         <v>1.0</v>
       </c>
       <c r="C4" t="n">
-        <v>20809.808203412336</v>
+        <v>0.3187909077606328</v>
       </c>
       <c r="D4" t="n">
-        <v>20809.808203412336</v>
+        <v>0.3187909077606328</v>
       </c>
       <c r="E4" t="n">
-        <v>0.21471235751107573</v>
+        <v>0.15329785520750586</v>
       </c>
       <c r="F4" t="n">
-        <v>0.001434311531804525</v>
+        <v>9.96425888652198E-4</v>
       </c>
       <c r="G4" t="n">
-        <v>0.6662</v>
+        <v>0.6966</v>
       </c>
     </row>
     <row r="5">
@@ -298,16 +298,16 @@
         <v>144.0</v>
       </c>
       <c r="C5" t="n">
-        <v>1.3956403888568915E7</v>
+        <v>299.4555315558221</v>
       </c>
       <c r="D5" t="n">
-        <v>96919.47144839524</v>
+        <v>2.079552302470987</v>
       </c>
       <c r="E5" t="e">
         <v>#N/A</v>
       </c>
       <c r="F5" t="n">
-        <v>0.9619421209568593</v>
+        <v>0.9359904466484088</v>
       </c>
       <c r="G5" t="e">
         <v>#N/A</v>
@@ -321,7 +321,7 @@
         <v>147.0</v>
       </c>
       <c r="C6" t="n">
-        <v>1.4508569262656111E7</v>
+        <v>319.9343888905185</v>
       </c>
       <c r="D6" t="e">
         <v>#N/A</v>
@@ -344,19 +344,19 @@
         <v>1.0</v>
       </c>
       <c r="C7" t="n">
-        <v>24.961229413456934</v>
+        <v>0.014985244785041773</v>
       </c>
       <c r="D7" t="n">
-        <v>24.961229413456934</v>
+        <v>0.014985244785041773</v>
       </c>
       <c r="E7" t="n">
-        <v>0.21212251719485045</v>
+        <v>0.018466824508721714</v>
       </c>
       <c r="F7" t="n">
-        <v>0.00145236208638025</v>
+        <v>1.2765746886156176E-4</v>
       </c>
       <c r="G7" t="n">
-        <v>0.6584</v>
+        <v>0.8936</v>
       </c>
     </row>
     <row r="8">
@@ -367,19 +367,19 @@
         <v>1.0</v>
       </c>
       <c r="C8" t="n">
-        <v>7.721344643873508</v>
+        <v>0.09824699122162449</v>
       </c>
       <c r="D8" t="n">
-        <v>7.721344643873508</v>
+        <v>0.09824699122162449</v>
       </c>
       <c r="E8" t="n">
-        <v>0.06561660224573819</v>
+        <v>0.12107309366148633</v>
       </c>
       <c r="F8" t="n">
-        <v>4.4926425821764117E-4</v>
+        <v>8.369541106953426E-4</v>
       </c>
       <c r="G8" t="n">
-        <v>0.8117</v>
+        <v>0.7284</v>
       </c>
     </row>
     <row r="9">
@@ -390,19 +390,19 @@
         <v>1.0</v>
       </c>
       <c r="C9" t="n">
-        <v>208.9562994176029</v>
+        <v>0.42166987486295987</v>
       </c>
       <c r="D9" t="n">
-        <v>208.9562994176029</v>
+        <v>0.42166987486295987</v>
       </c>
       <c r="E9" t="n">
-        <v>1.7757272881874537</v>
+        <v>0.5196380634023269</v>
       </c>
       <c r="F9" t="n">
-        <v>0.012158063289175802</v>
+        <v>0.0035921541284336706</v>
       </c>
       <c r="G9" t="n">
-        <v>0.1914</v>
+        <v>0.4741</v>
       </c>
     </row>
     <row r="10">
@@ -413,16 +413,16 @@
         <v>144.0</v>
       </c>
       <c r="C10" t="n">
-        <v>16945.004627849372</v>
+        <v>116.85145153282149</v>
       </c>
       <c r="D10" t="n">
-        <v>117.67364324895397</v>
+        <v>0.8114684134223714</v>
       </c>
       <c r="E10" t="e">
         <v>#N/A</v>
       </c>
       <c r="F10" t="n">
-        <v>0.9859403103662262</v>
+        <v>0.9954432342920094</v>
       </c>
       <c r="G10" t="e">
         <v>#N/A</v>
@@ -436,7 +436,7 @@
         <v>147.0</v>
       </c>
       <c r="C11" t="n">
-        <v>17186.643501324306</v>
+        <v>117.38635364369111</v>
       </c>
       <c r="D11" t="e">
         <v>#N/A</v>
@@ -459,19 +459,19 @@
         <v>1.0</v>
       </c>
       <c r="C12" t="n">
-        <v>1.4535097549956122</v>
+        <v>0.024329534532857605</v>
       </c>
       <c r="D12" t="n">
-        <v>1.4535097549956122</v>
+        <v>0.024329534532857605</v>
       </c>
       <c r="E12" t="n">
-        <v>0.02294710301059122</v>
+        <v>0.07103581191338554</v>
       </c>
       <c r="F12" t="n">
-        <v>1.5790309977683128E-4</v>
+        <v>4.8590278506825305E-4</v>
       </c>
       <c r="G12" t="n">
-        <v>0.8896</v>
+        <v>0.7934</v>
       </c>
     </row>
     <row r="13">
@@ -482,19 +482,19 @@
         <v>1.0</v>
       </c>
       <c r="C13" t="n">
-        <v>12.246102958330564</v>
+        <v>0.03956697516087168</v>
       </c>
       <c r="D13" t="n">
-        <v>12.246102958330564</v>
+        <v>0.03956697516087168</v>
       </c>
       <c r="E13" t="n">
-        <v>0.1933338149931891</v>
+        <v>0.11552511215179229</v>
       </c>
       <c r="F13" t="n">
-        <v>0.0013303643891350817</v>
+        <v>7.90220766510316E-4</v>
       </c>
       <c r="G13" t="n">
-        <v>0.6819</v>
+        <v>0.7376</v>
       </c>
     </row>
     <row r="14">
@@ -505,19 +505,19 @@
         <v>1.0</v>
       </c>
       <c r="C14" t="n">
-        <v>70.16203702199977</v>
+        <v>0.6873581967692158</v>
       </c>
       <c r="D14" t="n">
-        <v>70.16203702199977</v>
+        <v>0.6873581967692158</v>
       </c>
       <c r="E14" t="n">
-        <v>1.1076743623104226</v>
+        <v>2.0069043045965302</v>
       </c>
       <c r="F14" t="n">
-        <v>0.007622104423003342</v>
+        <v>0.013727729221395254</v>
       </c>
       <c r="G14" t="n">
-        <v>0.3093</v>
+        <v>0.1666</v>
       </c>
     </row>
     <row r="15">
@@ -528,16 +528,16 @@
         <v>144.0</v>
       </c>
       <c r="C15" t="n">
-        <v>9121.212582815504</v>
+        <v>49.31953163290764</v>
       </c>
       <c r="D15" t="n">
-        <v>63.341754047329886</v>
+        <v>0.3424967474507475</v>
       </c>
       <c r="E15" t="e">
         <v>#N/A</v>
       </c>
       <c r="F15" t="n">
-        <v>0.9908896280880849</v>
+        <v>0.9849961472270262</v>
       </c>
       <c r="G15" t="e">
         <v>#N/A</v>
@@ -551,7 +551,7 @@
         <v>147.0</v>
       </c>
       <c r="C16" t="n">
-        <v>9205.074232550829</v>
+        <v>50.070786339370585</v>
       </c>
       <c r="D16" t="e">
         <v>#N/A</v>
@@ -574,19 +574,19 @@
         <v>1.0</v>
       </c>
       <c r="C17" t="n">
-        <v>361.881547704592</v>
+        <v>1.8535900938485854E-4</v>
       </c>
       <c r="D17" t="n">
-        <v>361.881547704592</v>
+        <v>1.8535900938485854E-4</v>
       </c>
       <c r="E17" t="n">
-        <v>0.6668214129568691</v>
+        <v>2.4462077924020657E-4</v>
       </c>
       <c r="F17" t="n">
-        <v>0.004590771291725176</v>
+        <v>1.6791781192957105E-6</v>
       </c>
       <c r="G17" t="n">
-        <v>0.444</v>
+        <v>0.9889</v>
       </c>
     </row>
     <row r="18">
@@ -597,19 +597,19 @@
         <v>1.0</v>
       </c>
       <c r="C18" t="n">
-        <v>288.4236485069474</v>
+        <v>1.2000776516204612</v>
       </c>
       <c r="D18" t="n">
-        <v>288.4236485069474</v>
+        <v>1.2000776516204612</v>
       </c>
       <c r="E18" t="n">
-        <v>0.5314641380515395</v>
+        <v>1.583758627446219</v>
       </c>
       <c r="F18" t="n">
-        <v>0.0036588961604121202</v>
+        <v>0.010871573713867023</v>
       </c>
       <c r="G18" t="n">
-        <v>0.4912</v>
+        <v>0.2143</v>
       </c>
     </row>
     <row r="19">
@@ -620,19 +620,19 @@
         <v>1.0</v>
       </c>
       <c r="C19" t="n">
-        <v>29.469967626565108</v>
+        <v>0.07188809784372463</v>
       </c>
       <c r="D19" t="n">
-        <v>29.469967626565108</v>
+        <v>0.07188809784372463</v>
       </c>
       <c r="E19" t="n">
-        <v>0.0543028667175394</v>
+        <v>0.09487169019184793</v>
       </c>
       <c r="F19" t="n">
-        <v>3.7385128422890487E-4</v>
+        <v>6.512384876115563E-4</v>
       </c>
       <c r="G19" t="n">
-        <v>0.818</v>
+        <v>0.7615</v>
       </c>
     </row>
     <row r="20">
@@ -643,16 +643,16 @@
         <v>144.0</v>
       </c>
       <c r="C20" t="n">
-        <v>78148.27457082854</v>
+        <v>109.11459539260802</v>
       </c>
       <c r="D20" t="n">
-        <v>542.6963511863092</v>
+        <v>0.7577402457820002</v>
       </c>
       <c r="E20" t="e">
         <v>#N/A</v>
       </c>
       <c r="F20" t="n">
-        <v>0.9913764812636339</v>
+        <v>0.9884755086204021</v>
       </c>
       <c r="G20" t="e">
         <v>#N/A</v>
@@ -666,7 +666,7 @@
         <v>147.0</v>
       </c>
       <c r="C21" t="n">
-        <v>78828.04973466664</v>
+        <v>110.38674650108159</v>
       </c>
       <c r="D21" t="e">
         <v>#N/A</v>
@@ -689,19 +689,19 @@
         <v>1.0</v>
       </c>
       <c r="C22" t="n">
-        <v>7.5577514969399475</v>
+        <v>0.5151029099627621</v>
       </c>
       <c r="D22" t="n">
-        <v>7.5577514969399475</v>
+        <v>0.5151029099627621</v>
       </c>
       <c r="E22" t="n">
-        <v>5.320262029267417</v>
+        <v>3.035545453750894</v>
       </c>
       <c r="F22" t="n">
-        <v>0.03398585152895715</v>
+        <v>0.01979756498318349</v>
       </c>
       <c r="G22" t="n">
-        <v>0.0164</v>
+        <v>0.085</v>
       </c>
     </row>
     <row r="23">
@@ -712,19 +712,19 @@
         <v>1.0</v>
       </c>
       <c r="C23" t="n">
-        <v>6.324468090393808</v>
+        <v>0.6897191359769036</v>
       </c>
       <c r="D23" t="n">
-        <v>6.324468090393808</v>
+        <v>0.6897191359769036</v>
       </c>
       <c r="E23" t="n">
-        <v>4.4520949716670675</v>
+        <v>4.06457379114989</v>
       </c>
       <c r="F23" t="n">
-        <v>0.028439997478982876</v>
+        <v>0.026508798825529933</v>
       </c>
       <c r="G23" t="n">
-        <v>0.0299</v>
+        <v>0.0456</v>
       </c>
     </row>
     <row r="24">
@@ -735,19 +735,19 @@
         <v>1.0</v>
       </c>
       <c r="C24" t="n">
-        <v>3.9364863401004353</v>
+        <v>0.3782591923860461</v>
       </c>
       <c r="D24" t="n">
-        <v>3.9364863401004353</v>
+        <v>0.3782591923860461</v>
       </c>
       <c r="E24" t="n">
-        <v>2.7710806332340856</v>
+        <v>2.229113735486283</v>
       </c>
       <c r="F24" t="n">
-        <v>0.017701672296924473</v>
+        <v>0.014538087044180399</v>
       </c>
       <c r="G24" t="n">
-        <v>0.0971</v>
+        <v>0.1359</v>
       </c>
     </row>
     <row r="25">
@@ -758,16 +758,16 @@
         <v>144.0</v>
       </c>
       <c r="C25" t="n">
-        <v>204.56064185793684</v>
+        <v>24.43541701639917</v>
       </c>
       <c r="D25" t="n">
-        <v>1.4205600129023392</v>
+        <v>0.16969039594721647</v>
       </c>
       <c r="E25" t="e">
         <v>#N/A</v>
       </c>
       <c r="F25" t="n">
-        <v>0.9198724786951354</v>
+        <v>0.9391555491471062</v>
       </c>
       <c r="G25" t="e">
         <v>#N/A</v>
@@ -781,7 +781,7 @@
         <v>147.0</v>
       </c>
       <c r="C26" t="n">
-        <v>222.37934778537104</v>
+        <v>26.018498254724882</v>
       </c>
       <c r="D26" t="e">
         <v>#N/A</v>
@@ -804,19 +804,19 @@
         <v>1.0</v>
       </c>
       <c r="C27" t="n">
-        <v>43.13303023376838</v>
+        <v>0.024504662180262204</v>
       </c>
       <c r="D27" t="n">
-        <v>43.13303023376838</v>
+        <v>0.024504662180262204</v>
       </c>
       <c r="E27" t="n">
-        <v>1.9942961243538564</v>
+        <v>0.05037321734871641</v>
       </c>
       <c r="F27" t="n">
-        <v>0.013608081587372355</v>
+        <v>3.488594343584305E-4</v>
       </c>
       <c r="G27" t="n">
-        <v>0.1599</v>
+        <v>0.8171</v>
       </c>
     </row>
     <row r="28">
@@ -827,19 +827,19 @@
         <v>1.0</v>
       </c>
       <c r="C28" t="n">
-        <v>5.415171167745356</v>
+        <v>0.05079873230225809</v>
       </c>
       <c r="D28" t="n">
-        <v>5.415171167745356</v>
+        <v>0.05079873230225809</v>
       </c>
       <c r="E28" t="n">
-        <v>0.25037551996735286</v>
+        <v>0.10442484636095184</v>
       </c>
       <c r="F28" t="n">
-        <v>0.001708437609434963</v>
+        <v>7.231936880715433E-4</v>
       </c>
       <c r="G28" t="n">
-        <v>0.6252</v>
+        <v>0.7444</v>
       </c>
     </row>
     <row r="29">
@@ -850,19 +850,19 @@
         <v>1.0</v>
       </c>
       <c r="C29" t="n">
-        <v>6.654192428913433</v>
+        <v>0.11637409341924573</v>
       </c>
       <c r="D29" t="n">
-        <v>6.654192428913433</v>
+        <v>0.11637409341924573</v>
       </c>
       <c r="E29" t="n">
-        <v>0.30766283054459637</v>
+        <v>0.23922539549593444</v>
       </c>
       <c r="F29" t="n">
-        <v>0.00209933763011712</v>
+        <v>0.001656754135419744</v>
       </c>
       <c r="G29" t="n">
-        <v>0.6053</v>
+        <v>0.6292</v>
       </c>
     </row>
     <row r="30">
@@ -873,16 +873,16 @@
         <v>144.0</v>
       </c>
       <c r="C30" t="n">
-        <v>3114.4604243138847</v>
+        <v>70.05054550178883</v>
       </c>
       <c r="D30" t="n">
-        <v>21.628197391068642</v>
+        <v>0.48646212154020024</v>
       </c>
       <c r="E30" t="e">
         <v>#N/A</v>
       </c>
       <c r="F30" t="n">
-        <v>0.9825841431730755</v>
+        <v>0.9972711927421503</v>
       </c>
       <c r="G30" t="e">
         <v>#N/A</v>
@@ -896,7 +896,7 @@
         <v>147.0</v>
       </c>
       <c r="C31" t="n">
-        <v>3169.662818144312</v>
+        <v>70.2422229896906</v>
       </c>
       <c r="D31" t="e">
         <v>#N/A</v>
@@ -919,19 +919,19 @@
         <v>1.0</v>
       </c>
       <c r="C32" t="n">
-        <v>285.3767893741314</v>
+        <v>0.02198466568461665</v>
       </c>
       <c r="D32" t="n">
-        <v>285.3767893741314</v>
+        <v>0.02198466568461665</v>
       </c>
       <c r="E32" t="n">
-        <v>0.06942416747338381</v>
+        <v>0.018768248912625986</v>
       </c>
       <c r="F32" t="n">
-        <v>4.644794693235082E-4</v>
+        <v>1.1972302791403514E-4</v>
       </c>
       <c r="G32" t="n">
-        <v>0.8103</v>
+        <v>0.8915</v>
       </c>
     </row>
     <row r="33">
@@ -942,19 +942,19 @@
         <v>1.0</v>
       </c>
       <c r="C33" t="n">
-        <v>22039.838295957987</v>
+        <v>14.916104555775465</v>
       </c>
       <c r="D33" t="n">
-        <v>22039.838295957987</v>
+        <v>14.916104555775465</v>
       </c>
       <c r="E33" t="n">
-        <v>5.36167439650782</v>
+        <v>12.733837626898165</v>
       </c>
       <c r="F33" t="n">
-        <v>0.03587205679247318</v>
+        <v>0.0812293999698778</v>
       </c>
       <c r="G33" t="n">
-        <v>0.0145</v>
+        <v>6.0E-4</v>
       </c>
     </row>
     <row r="34">
@@ -965,19 +965,19 @@
         <v>1.0</v>
       </c>
       <c r="C34" t="n">
-        <v>145.93687728609802</v>
+        <v>0.01323100014625389</v>
       </c>
       <c r="D34" t="n">
-        <v>145.93687728609802</v>
+        <v>0.01323100014625389</v>
       </c>
       <c r="E34" t="n">
-        <v>0.03550234842669769</v>
+        <v>0.011295268605409949</v>
       </c>
       <c r="F34" t="n">
-        <v>2.3752696729554428E-4</v>
+        <v>7.205273996724773E-5</v>
       </c>
       <c r="G34" t="n">
-        <v>0.8611</v>
+        <v>0.9142</v>
       </c>
     </row>
     <row r="35">
@@ -988,16 +988,16 @@
         <v>144.0</v>
       </c>
       <c r="C35" t="n">
-        <v>591930.1471728826</v>
+        <v>168.67806225945088</v>
       </c>
       <c r="D35" t="n">
-        <v>4110.626022033906</v>
+        <v>1.1713754323572978</v>
       </c>
       <c r="E35" t="e">
         <v>#N/A</v>
       </c>
       <c r="F35" t="n">
-        <v>0.9634259367709077</v>
+        <v>0.918578824262241</v>
       </c>
       <c r="G35" t="e">
         <v>#N/A</v>
@@ -1011,7 +1011,7 @@
         <v>147.0</v>
       </c>
       <c r="C36" t="n">
-        <v>614401.2991355008</v>
+        <v>183.6293824810572</v>
       </c>
       <c r="D36" t="e">
         <v>#N/A</v>
@@ -1034,19 +1034,19 @@
         <v>1.0</v>
       </c>
       <c r="C37" t="n">
-        <v>62.426868342683825</v>
+        <v>0.07071000669817332</v>
       </c>
       <c r="D37" t="n">
-        <v>62.426868342683825</v>
+        <v>0.07071000669817332</v>
       </c>
       <c r="E37" t="n">
-        <v>0.11014473850854847</v>
+        <v>0.2027099944885343</v>
       </c>
       <c r="F37" t="n">
-        <v>7.422673556148049E-4</v>
+        <v>0.0013579457065837552</v>
       </c>
       <c r="G37" t="n">
-        <v>0.6948</v>
+        <v>0.6929</v>
       </c>
     </row>
     <row r="38">
@@ -1057,19 +1057,19 @@
         <v>1.0</v>
       </c>
       <c r="C38" t="n">
-        <v>2366.31750570481</v>
+        <v>1.703025948354592</v>
       </c>
       <c r="D38" t="n">
-        <v>2366.31750570481</v>
+        <v>1.703025948354592</v>
       </c>
       <c r="E38" t="n">
-        <v>4.175084059372051</v>
+        <v>4.882199800635975</v>
       </c>
       <c r="F38" t="n">
-        <v>0.028135965877109037</v>
+        <v>0.03270565062509871</v>
       </c>
       <c r="G38" t="n">
-        <v>0.0498</v>
+        <v>0.0528</v>
       </c>
     </row>
     <row r="39">
@@ -1080,19 +1080,19 @@
         <v>1.0</v>
       </c>
       <c r="C39" t="n">
-        <v>59.14124369306728</v>
+        <v>0.06698842739827304</v>
       </c>
       <c r="D39" t="n">
-        <v>59.14124369306728</v>
+        <v>0.06698842739827304</v>
       </c>
       <c r="E39" t="n">
-        <v>0.10434764700809572</v>
+        <v>0.19204104741020064</v>
       </c>
       <c r="F39" t="n">
-        <v>7.032006526876909E-4</v>
+        <v>0.0012864748799215212</v>
       </c>
       <c r="G39" t="n">
-        <v>0.7419</v>
+        <v>0.7341</v>
       </c>
     </row>
     <row r="40">
@@ -1103,16 +1103,16 @@
         <v>144.0</v>
       </c>
       <c r="C40" t="n">
-        <v>81615.05636194132</v>
+        <v>50.230581823201064</v>
       </c>
       <c r="D40" t="n">
-        <v>566.7712247357035</v>
+        <v>0.3488234848833407</v>
       </c>
       <c r="E40" t="e">
         <v>#N/A</v>
       </c>
       <c r="F40" t="n">
-        <v>0.9704185661145885</v>
+        <v>0.9646499287883961</v>
       </c>
       <c r="G40" t="e">
         <v>#N/A</v>
@@ -1126,7 +1126,7 @@
         <v>147.0</v>
       </c>
       <c r="C41" t="n">
-        <v>84102.94197968187</v>
+        <v>52.0713062056521</v>
       </c>
       <c r="D41" t="e">
         <v>#N/A</v>

</xml_diff>